<commit_message>
Fix #139, minor bugfix and work on documentation
</commit_message>
<xml_diff>
--- a/sbmlutils/tests/data/models/demo/demo_annotations.xlsx
+++ b/sbmlutils/tests/data/models/demo/demo_annotations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Annotation" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="64">
   <si>
     <t xml:space="preserve">pattern</t>
   </si>
@@ -34,9 +34,6 @@
     <t xml:space="preserve">qualifier</t>
   </si>
   <si>
-    <t xml:space="preserve">collection</t>
-  </si>
-  <si>
     <t xml:space="preserve">resource</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t xml:space="preserve">BQM_IS</t>
   </si>
   <si>
-    <t xml:space="preserve">sbo</t>
-  </si>
-  <si>
     <t xml:space="preserve">sbo/SBO:0000293</t>
   </si>
   <si>
@@ -70,9 +64,6 @@
     <t xml:space="preserve">model</t>
   </si>
   <si>
-    <t xml:space="preserve">go</t>
-  </si>
-  <si>
     <t xml:space="preserve">go/GO:0008152</t>
   </si>
   <si>
@@ -101,9 +92,6 @@
   </si>
   <si>
     <t xml:space="preserve">extracellular space</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fma</t>
   </si>
   <si>
     <t xml:space="preserve">fma/FMA:70022</t>
@@ -399,12 +387,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -474,22 +462,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="19.1428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.1428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="32.6938775510204"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="1" width="19.1428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="19.1428571428571"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="32.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="7" style="1" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1023" style="0" width="19.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -505,69 +493,59 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,86 +555,75 @@
       <c r="D5" s="0"/>
       <c r="E5" s="0"/>
       <c r="F5" s="0"/>
-      <c r="G5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="F7" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="F8" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -666,75 +633,65 @@
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -744,75 +701,65 @@
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -820,88 +767,77 @@
       <c r="B18" s="0"/>
       <c r="C18" s="0"/>
       <c r="D18" s="0"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="0"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="F21" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -911,183 +847,163 @@
       <c r="D23" s="0"/>
       <c r="E23" s="0"/>
       <c r="F23" s="0"/>
-      <c r="G23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="5"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>52</v>
+        <v>19</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>52</v>
+        <v>19</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>52</v>
+        <v>19</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D28" s="0"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G28" s="0"/>
+      <c r="E28" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G29" s="0"/>
+      <c r="F29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="5"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>64</v>
+        <v>19</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B32" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>67</v>
+      <c r="F32" s="15" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Extended available types for annotation from tabular format by fbc:geneProduct tag.
</commit_message>
<xml_diff>
--- a/sbmlutils/tests/data/models/demo/demo_annotations.xlsx
+++ b/sbmlutils/tests/data/models/demo/demo_annotations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="69">
   <si>
     <t xml:space="preserve">pattern</t>
   </si>
@@ -212,6 +212,21 @@
   </si>
   <si>
     <t xml:space="preserve">biochemical reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># fbc:geneProducts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^PSHA_RS08100$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fbc:geneProduct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://identifiers.org/ncbigene/3708256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acetyl-CoA:oxaloacetate C-acetyltransferase</t>
   </si>
 </sst>
 </file>
@@ -387,12 +402,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -462,10 +477,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -474,7 +489,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="32.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="32.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="7" style="1" width="19.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1023" style="0" width="19.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
@@ -998,6 +1013,36 @@
       </c>
       <c r="F32" s="15" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>